<commit_message>
Temperature Sensor Rev 1 Design Files Update
- Updated CAD files to most recent version
- Updated user manual to reflect CAD
- Updated 3D printing STL and STEP files
</commit_message>
<xml_diff>
--- a/Temperature Sensor Rev 1.0/FPR05-00_1_BOM_Temperature Sensor Module.xlsx
+++ b/Temperature Sensor Rev 1.0/FPR05-00_1_BOM_Temperature Sensor Module.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Shared Folders\a_Project\FP05_Prop_YY_NN_Internal Projects\FP05 - Temperature Sensor Module\d_Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fprin-my.sharepoint.com/personal/lparrish_fprin_com/Documents/Documents/GitHub/FPrin_Temperature_Sensor_Module/Temperature Sensor Rev 1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDB1DA5-6D29-46E7-AD3D-D83280D0B03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1DDB1DA5-6D29-46E7-AD3D-D83280D0B03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB122F1A-6CA3-4442-A7D4-49C0198D60D5}"/>
   <bookViews>
-    <workbookView xWindow="-51600" yWindow="-15870" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33585" yWindow="-8325" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t xml:space="preserve">ASSY NO: </t>
   </si>
@@ -83,9 +83,6 @@
     <t>95495K18</t>
   </si>
   <si>
-    <t>5862K141</t>
-  </si>
-  <si>
     <t>FPR12090</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
   </si>
   <si>
     <t>Rubber Feet</t>
-  </si>
-  <si>
-    <t>Neodymium Magnets</t>
   </si>
   <si>
     <t>2k Through-hole Resistor</t>
@@ -167,9 +161,6 @@
   </si>
   <si>
     <t>https://www.amazon.com/gp/product/B07WXKWNQF/ref=ppx_yo_dt_b_asin_title_o02_s00?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/5862K141/</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/95495k18/</t>
@@ -372,8 +363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83009126-9426-48AD-9D65-B42C7EAEAF75}" name="Table1" displayName="Table1" ref="A6:G18" totalsRowShown="0">
-  <autoFilter ref="A6:G18" xr:uid="{83009126-9426-48AD-9D65-B42C7EAEAF75}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83009126-9426-48AD-9D65-B42C7EAEAF75}" name="Table1" displayName="Table1" ref="A6:G17" totalsRowShown="0">
+  <autoFilter ref="A6:G17" xr:uid="{83009126-9426-48AD-9D65-B42C7EAEAF75}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A1B8B3ED-C911-4344-8DE1-2429F246AD27}" name="Item"/>
     <tableColumn id="2" xr3:uid="{FFA8AA5E-BCD5-419D-B939-60252BE7ECBF}" name="Qty"/>
@@ -650,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,13 +699,13 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="8">
         <f>SUMPRODUCT(Table1[Qty],Table1[Unit Cost])</f>
-        <v>60.83</v>
+        <v>59.29</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -734,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
@@ -750,19 +741,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="7">
         <v>7.59</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
@@ -776,19 +767,19 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="7">
         <v>26.4</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
@@ -802,19 +793,19 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7">
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
@@ -831,16 +822,16 @@
         <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -854,19 +845,19 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
@@ -883,16 +874,16 @@
         <v>14</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7">
         <v>4.13</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
@@ -906,16 +897,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="7">
-        <v>0.77</v>
+        <v>0.1</v>
       </c>
       <c r="G13" t="s">
         <v>40</v>
@@ -929,22 +920,22 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.54</v>
+      </c>
+      <c r="G14" t="s">
         <v>42</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>43</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
@@ -958,19 +949,19 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F15" s="7">
-        <v>0.54</v>
+        <v>0.49</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
@@ -984,19 +975,19 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>26</v>
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="7">
-        <v>0.49</v>
+        <v>0.32</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
@@ -1010,46 +1001,25 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
+        <v>48</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F17" s="7">
-        <v>0.32</v>
+        <v>8.6199999999999992</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="7">
-        <v>8.6199999999999992</v>
-      </c>
-      <c r="G18" t="s">
-        <v>53</v>
-      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
@@ -1174,11 +1144,7 @@
       <c r="J42" s="5"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="9:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I43" s="4"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="4"/>
-    </row>
+    <row r="43" spans="9:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="9:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="9:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="9:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1163,6 @@
     <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:C1"/>

</xml_diff>